<commit_message>
chore: Update trial variables in ODU_GT.ino
</commit_message>
<xml_diff>
--- a/Arduino_code/ODU_GT/trial_time_calculator.xlsx
+++ b/Arduino_code/ODU_GT/trial_time_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\context-project\Arduino_code\ODU_GT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5492DB6-8EA7-4713-A189-390045B6B841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B109F0-2795-4BB1-8A1E-D8292819AE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4164" yWindow="5292" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,15 +125,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -419,7 +418,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,47 +438,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -488,39 +487,39 @@
         <v>60</v>
       </c>
       <c r="B3" s="1">
-        <v>560</v>
+        <v>330</v>
       </c>
       <c r="C3" s="1">
         <v>60</v>
       </c>
       <c r="D3" s="1">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2">
+        <v>60</v>
+      </c>
+      <c r="G3">
         <f>A3+C3+6*(B3+D3+E3+F3)</f>
-        <v>3552</v>
-      </c>
-      <c r="H3" s="2">
+        <v>3600</v>
+      </c>
+      <c r="H3">
         <f>INT(G3/3600)</f>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>INT((G3-H3*3600)/60)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="2">
-        <f>INT((G3-H3*3600)/60)</f>
-        <v>59</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <f>MOD(G3, 60)</f>
-        <v>12</v>
-      </c>
-      <c r="K3" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="K3" t="str">
         <f>H3 &amp; " hours " &amp; I3 &amp; " minutes " &amp; J3 &amp; " seconds"</f>
-        <v>0 hours 59 minutes 12 seconds</v>
+        <v>1 hours 0 minutes 0 seconds</v>
       </c>
     </row>
   </sheetData>

</xml_diff>